<commit_message>
Fixed small issues with excel sheets
</commit_message>
<xml_diff>
--- a/PythonApplication1/2022_Wholesale_Prices.xlsx
+++ b/PythonApplication1/2022_Wholesale_Prices.xlsx
@@ -1508,502 +1508,534 @@
       <c r="B5" s="4" t="n"/>
       <c r="C5" s="51" t="inlineStr">
         <is>
+          <t>Premium Bark</t>
+        </is>
+      </c>
+      <c r="D5" s="32" t="inlineStr">
+        <is>
           <t>27.00</t>
         </is>
       </c>
-      <c r="D5" s="32" t="inlineStr">
+      <c r="E5" s="32" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="E5" s="32" t="inlineStr">
+      <c r="F5" s="32" t="inlineStr">
         <is>
           <t>24.75</t>
         </is>
       </c>
-      <c r="F5" s="32" t="inlineStr">
+      <c r="G5" s="33" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="G5" s="33" t="n"/>
       <c r="H5" s="66" t="inlineStr">
         <is>
+          <t>Premium Bark</t>
+        </is>
+      </c>
+      <c r="I5" s="17" t="inlineStr">
+        <is>
           <t>50.75</t>
         </is>
       </c>
-      <c r="I5" s="17" t="inlineStr">
+      <c r="J5" s="17" t="inlineStr">
         <is>
           <t>44.75</t>
         </is>
       </c>
-      <c r="J5" s="17" t="inlineStr">
+      <c r="K5" s="17" t="inlineStr">
         <is>
           <t>40.75</t>
         </is>
       </c>
-      <c r="K5" s="17" t="inlineStr">
+      <c r="L5" s="17" t="inlineStr">
         <is>
           <t>39.00</t>
         </is>
       </c>
-      <c r="L5" s="17" t="inlineStr">
+      <c r="M5" s="17" t="inlineStr">
         <is>
           <t>37.75</t>
         </is>
       </c>
-      <c r="M5" s="17" t="inlineStr">
+      <c r="N5" s="17" t="inlineStr">
         <is>
           <t>36.00</t>
         </is>
       </c>
-      <c r="N5" s="17" t="inlineStr">
+      <c r="O5" s="17" t="inlineStr">
         <is>
           <t>35.75</t>
         </is>
       </c>
-      <c r="O5" s="17" t="inlineStr">
+      <c r="P5" s="17" t="inlineStr">
         <is>
           <t>35.50</t>
         </is>
       </c>
-      <c r="P5" s="17" t="inlineStr">
+      <c r="Q5" s="17" t="inlineStr">
         <is>
           <t>34.50</t>
         </is>
       </c>
-      <c r="Q5" s="17" t="inlineStr">
+      <c r="R5" s="17" t="inlineStr">
         <is>
           <t>33.75</t>
         </is>
       </c>
-      <c r="R5" s="17" t="inlineStr">
+      <c r="S5" s="17" t="inlineStr">
         <is>
           <t>33.00</t>
         </is>
       </c>
-      <c r="S5" s="17" t="inlineStr">
+      <c r="T5" s="17" t="inlineStr">
         <is>
           <t>32.50</t>
         </is>
       </c>
-      <c r="T5" s="17" t="inlineStr">
+      <c r="U5" s="17" t="inlineStr">
         <is>
           <t>32.00</t>
         </is>
       </c>
-      <c r="U5" s="17" t="inlineStr">
+      <c r="V5" s="17" t="inlineStr">
         <is>
           <t>31.75</t>
         </is>
       </c>
-      <c r="V5" s="17" t="inlineStr">
+      <c r="W5" s="17" t="inlineStr">
         <is>
           <t>31.25</t>
         </is>
       </c>
-      <c r="W5" s="17" t="inlineStr">
+      <c r="X5" s="17" t="inlineStr">
         <is>
           <t>30.25</t>
         </is>
       </c>
-      <c r="X5" s="17" t="inlineStr">
+      <c r="Y5" s="17" t="inlineStr">
         <is>
           <t>29.25</t>
         </is>
       </c>
-      <c r="Y5" s="17" t="inlineStr">
+      <c r="Z5" s="17" t="inlineStr">
         <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="Z5" s="17" t="inlineStr">
+      <c r="AA5" s="17" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="AA5" s="17" t="inlineStr">
+      <c r="AB5" s="18" t="inlineStr">
         <is>
           <t>27.00</t>
         </is>
       </c>
-      <c r="AB5" s="18" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="6">
       <c r="B6" s="4" t="n"/>
       <c r="C6" s="52" t="inlineStr">
         <is>
+          <t>Bark Blend</t>
+        </is>
+      </c>
+      <c r="D6" s="34" t="inlineStr">
+        <is>
           <t>23.00</t>
         </is>
       </c>
-      <c r="D6" s="34" t="inlineStr">
+      <c r="E6" s="34" t="inlineStr">
         <is>
           <t>22.25</t>
         </is>
       </c>
-      <c r="E6" s="34" t="inlineStr">
+      <c r="F6" s="34" t="inlineStr">
         <is>
           <t>20.75</t>
         </is>
       </c>
-      <c r="F6" s="34" t="inlineStr">
+      <c r="G6" s="20" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="G6" s="20" t="n"/>
       <c r="H6" s="67" t="inlineStr">
         <is>
+          <t>Bark Blend</t>
+        </is>
+      </c>
+      <c r="I6" s="19" t="inlineStr">
+        <is>
           <t>46.75</t>
         </is>
       </c>
-      <c r="I6" s="19" t="inlineStr">
+      <c r="J6" s="19" t="inlineStr">
         <is>
           <t>40.75</t>
         </is>
       </c>
-      <c r="J6" s="19" t="inlineStr">
+      <c r="K6" s="19" t="inlineStr">
         <is>
           <t>36.75</t>
         </is>
       </c>
-      <c r="K6" s="19" t="inlineStr">
+      <c r="L6" s="19" t="inlineStr">
         <is>
           <t>35.00</t>
         </is>
       </c>
-      <c r="L6" s="19" t="inlineStr">
+      <c r="M6" s="19" t="inlineStr">
         <is>
           <t>33.75</t>
         </is>
       </c>
-      <c r="M6" s="19" t="inlineStr">
+      <c r="N6" s="19" t="inlineStr">
         <is>
           <t>32.00</t>
         </is>
       </c>
-      <c r="N6" s="19" t="inlineStr">
+      <c r="O6" s="19" t="inlineStr">
         <is>
           <t>31.75</t>
         </is>
       </c>
-      <c r="O6" s="19" t="inlineStr">
+      <c r="P6" s="19" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="P6" s="19" t="inlineStr">
+      <c r="Q6" s="19" t="inlineStr">
         <is>
           <t>30.50</t>
         </is>
       </c>
-      <c r="Q6" s="19" t="inlineStr">
+      <c r="R6" s="19" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="R6" s="19" t="inlineStr">
+      <c r="S6" s="19" t="inlineStr">
         <is>
           <t>29.00</t>
         </is>
       </c>
-      <c r="S6" s="19" t="inlineStr">
+      <c r="T6" s="19" t="inlineStr">
         <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="T6" s="19" t="inlineStr">
+      <c r="U6" s="19" t="inlineStr">
         <is>
           <t>28.00</t>
         </is>
       </c>
-      <c r="U6" s="19" t="inlineStr">
+      <c r="V6" s="19" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="V6" s="19" t="inlineStr">
+      <c r="W6" s="19" t="inlineStr">
         <is>
           <t>27.25</t>
         </is>
       </c>
-      <c r="W6" s="19" t="inlineStr">
+      <c r="X6" s="19" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="X6" s="19" t="inlineStr">
+      <c r="Y6" s="19" t="inlineStr">
         <is>
           <t>25.25</t>
         </is>
       </c>
-      <c r="Y6" s="19" t="inlineStr">
+      <c r="Z6" s="19" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="Z6" s="19" t="inlineStr">
+      <c r="AA6" s="19" t="inlineStr">
         <is>
           <t>23.75</t>
         </is>
       </c>
-      <c r="AA6" s="19" t="inlineStr">
+      <c r="AB6" s="20" t="inlineStr">
         <is>
           <t>23.00</t>
         </is>
       </c>
-      <c r="AB6" s="20" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="6" t="n"/>
       <c r="C7" s="53" t="inlineStr">
         <is>
+          <t>Nature's Blend</t>
+        </is>
+      </c>
+      <c r="D7" s="35" t="inlineStr">
+        <is>
           <t>19.00</t>
         </is>
       </c>
-      <c r="D7" s="35" t="inlineStr">
+      <c r="E7" s="35" t="inlineStr">
         <is>
           <t>18.25</t>
         </is>
       </c>
-      <c r="E7" s="35" t="inlineStr">
+      <c r="F7" s="35" t="inlineStr">
         <is>
           <t>16.75</t>
         </is>
       </c>
-      <c r="F7" s="35" t="inlineStr">
+      <c r="G7" s="22" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="G7" s="22" t="n"/>
       <c r="H7" s="68" t="inlineStr">
         <is>
+          <t>Nature's Blend</t>
+        </is>
+      </c>
+      <c r="I7" s="21" t="inlineStr">
+        <is>
           <t>42.75</t>
         </is>
       </c>
-      <c r="I7" s="21" t="inlineStr">
+      <c r="J7" s="21" t="inlineStr">
         <is>
           <t>36.75</t>
         </is>
       </c>
-      <c r="J7" s="21" t="inlineStr">
+      <c r="K7" s="21" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="K7" s="21" t="inlineStr">
+      <c r="L7" s="21" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="L7" s="21" t="inlineStr">
+      <c r="M7" s="21" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="M7" s="21" t="inlineStr">
+      <c r="N7" s="21" t="inlineStr">
         <is>
           <t>28.00</t>
         </is>
       </c>
-      <c r="N7" s="21" t="inlineStr">
+      <c r="O7" s="21" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="O7" s="21" t="inlineStr">
+      <c r="P7" s="21" t="inlineStr">
         <is>
           <t>27.50</t>
         </is>
       </c>
-      <c r="P7" s="21" t="inlineStr">
+      <c r="Q7" s="21" t="inlineStr">
         <is>
           <t>26.50</t>
         </is>
       </c>
-      <c r="Q7" s="21" t="inlineStr">
+      <c r="R7" s="21" t="inlineStr">
         <is>
           <t>25.75</t>
         </is>
       </c>
-      <c r="R7" s="21" t="inlineStr">
+      <c r="S7" s="21" t="inlineStr">
         <is>
           <t>25.00</t>
         </is>
       </c>
-      <c r="S7" s="21" t="inlineStr">
+      <c r="T7" s="21" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="T7" s="21" t="inlineStr">
+      <c r="U7" s="21" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="U7" s="21" t="inlineStr">
+      <c r="V7" s="21" t="inlineStr">
         <is>
           <t>23.75</t>
         </is>
       </c>
-      <c r="V7" s="21" t="inlineStr">
+      <c r="W7" s="21" t="inlineStr">
         <is>
           <t>23.25</t>
         </is>
       </c>
-      <c r="W7" s="21" t="inlineStr">
+      <c r="X7" s="21" t="inlineStr">
         <is>
           <t>22.25</t>
         </is>
       </c>
-      <c r="X7" s="21" t="inlineStr">
+      <c r="Y7" s="21" t="inlineStr">
         <is>
           <t>21.25</t>
         </is>
       </c>
-      <c r="Y7" s="21" t="inlineStr">
+      <c r="Z7" s="21" t="inlineStr">
         <is>
           <t>20.50</t>
         </is>
       </c>
-      <c r="Z7" s="21" t="inlineStr">
+      <c r="AA7" s="21" t="inlineStr">
         <is>
           <t>19.75</t>
         </is>
       </c>
-      <c r="AA7" s="21" t="inlineStr">
+      <c r="AB7" s="22" t="inlineStr">
         <is>
           <t>19.00</t>
         </is>
       </c>
-      <c r="AB7" s="22" t="n"/>
     </row>
     <row customHeight="1" ht="56.25" r="8">
       <c r="B8" s="4" t="n"/>
       <c r="C8" s="54" t="inlineStr">
         <is>
+          <t>Beauty Bark</t>
+        </is>
+      </c>
+      <c r="D8" s="83" t="inlineStr">
+        <is>
           <t>32.50</t>
         </is>
       </c>
-      <c r="D8" s="83" t="inlineStr">
+      <c r="E8" s="83" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="E8" s="83" t="inlineStr">
+      <c r="F8" s="83" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="F8" s="83" t="inlineStr">
+      <c r="G8" s="84" t="inlineStr">
         <is>
           <t>29.00</t>
         </is>
       </c>
-      <c r="G8" s="84" t="n"/>
       <c r="H8" s="69" t="inlineStr">
         <is>
+          <t>Beauty Bark</t>
+        </is>
+      </c>
+      <c r="I8" s="85" t="inlineStr">
+        <is>
           <t>56.50</t>
         </is>
       </c>
-      <c r="I8" s="85" t="inlineStr">
+      <c r="J8" s="86" t="inlineStr">
         <is>
           <t>50.25</t>
         </is>
       </c>
-      <c r="J8" s="86" t="inlineStr">
+      <c r="K8" s="86" t="inlineStr">
         <is>
           <t>46.25</t>
         </is>
       </c>
-      <c r="K8" s="86" t="inlineStr">
+      <c r="L8" s="86" t="inlineStr">
         <is>
           <t>44.50</t>
         </is>
       </c>
-      <c r="L8" s="86" t="inlineStr">
+      <c r="M8" s="86" t="inlineStr">
         <is>
           <t>43.25</t>
         </is>
       </c>
-      <c r="M8" s="86" t="inlineStr">
+      <c r="N8" s="86" t="inlineStr">
         <is>
           <t>41.00</t>
         </is>
       </c>
-      <c r="N8" s="86" t="inlineStr">
+      <c r="O8" s="86" t="inlineStr">
         <is>
           <t>40.75</t>
         </is>
       </c>
-      <c r="O8" s="86" t="inlineStr">
+      <c r="P8" s="86" t="inlineStr">
         <is>
           <t>40.50</t>
         </is>
       </c>
-      <c r="P8" s="86" t="inlineStr">
+      <c r="Q8" s="86" t="inlineStr">
         <is>
           <t>39.50</t>
         </is>
       </c>
-      <c r="Q8" s="86" t="inlineStr">
+      <c r="R8" s="86" t="inlineStr">
         <is>
           <t>38.75</t>
         </is>
       </c>
-      <c r="R8" s="86" t="inlineStr">
+      <c r="S8" s="86" t="inlineStr">
         <is>
           <t>38.00</t>
         </is>
       </c>
-      <c r="S8" s="86" t="inlineStr">
+      <c r="T8" s="86" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="T8" s="86" t="inlineStr">
+      <c r="U8" s="86" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="U8" s="86" t="inlineStr">
+      <c r="V8" s="86" t="inlineStr">
         <is>
           <t>36.75</t>
         </is>
       </c>
-      <c r="V8" s="86" t="inlineStr">
+      <c r="W8" s="86" t="inlineStr">
         <is>
           <t>36.25</t>
         </is>
       </c>
-      <c r="W8" s="86" t="inlineStr">
+      <c r="X8" s="86" t="inlineStr">
         <is>
           <t>35.25</t>
         </is>
       </c>
-      <c r="X8" s="86" t="inlineStr">
+      <c r="Y8" s="86" t="inlineStr">
         <is>
           <t>34.25</t>
         </is>
       </c>
-      <c r="Y8" s="86" t="inlineStr">
+      <c r="Z8" s="86" t="inlineStr">
         <is>
           <t>33.50</t>
         </is>
       </c>
-      <c r="Z8" s="86" t="inlineStr">
+      <c r="AA8" s="86" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="AA8" s="86" t="inlineStr">
+      <c r="AB8" s="87" t="inlineStr">
         <is>
           <t>32.00</t>
         </is>
       </c>
-      <c r="AB8" s="87" t="n"/>
     </row>
     <row customHeight="1" ht="37.5" r="9">
       <c r="B9" s="4" t="n"/>
@@ -2046,126 +2078,134 @@
       <c r="B10" s="4" t="n"/>
       <c r="C10" s="56" t="inlineStr">
         <is>
+          <t>Dyed Mulch</t>
+        </is>
+      </c>
+      <c r="D10" s="88" t="inlineStr">
+        <is>
           <t>25.50</t>
         </is>
       </c>
-      <c r="D10" s="88" t="inlineStr">
+      <c r="E10" s="88" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="E10" s="88" t="inlineStr">
+      <c r="F10" s="88" t="inlineStr">
         <is>
           <t>22.75</t>
         </is>
       </c>
-      <c r="F10" s="88" t="inlineStr">
+      <c r="G10" s="89" t="inlineStr">
         <is>
           <t>22.00</t>
         </is>
       </c>
-      <c r="G10" s="89" t="n"/>
       <c r="H10" s="71" t="inlineStr">
         <is>
+          <t>Dyed Mulch</t>
+        </is>
+      </c>
+      <c r="I10" s="88" t="inlineStr">
+        <is>
           <t>49.50</t>
         </is>
       </c>
-      <c r="I10" s="88" t="inlineStr">
+      <c r="J10" s="88" t="inlineStr">
         <is>
           <t>43.25</t>
         </is>
       </c>
-      <c r="J10" s="88" t="inlineStr">
+      <c r="K10" s="88" t="inlineStr">
         <is>
           <t>39.25</t>
         </is>
       </c>
-      <c r="K10" s="88" t="inlineStr">
+      <c r="L10" s="88" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="L10" s="88" t="inlineStr">
+      <c r="M10" s="88" t="inlineStr">
         <is>
           <t>36.25</t>
         </is>
       </c>
-      <c r="M10" s="88" t="inlineStr">
+      <c r="N10" s="88" t="inlineStr">
         <is>
           <t>34.00</t>
         </is>
       </c>
-      <c r="N10" s="88" t="inlineStr">
+      <c r="O10" s="88" t="inlineStr">
         <is>
           <t>33.75</t>
         </is>
       </c>
-      <c r="O10" s="88" t="inlineStr">
+      <c r="P10" s="88" t="inlineStr">
         <is>
           <t>33.50</t>
         </is>
       </c>
-      <c r="P10" s="88" t="inlineStr">
+      <c r="Q10" s="88" t="inlineStr">
         <is>
           <t>32.50</t>
         </is>
       </c>
-      <c r="Q10" s="88" t="inlineStr">
+      <c r="R10" s="88" t="inlineStr">
         <is>
           <t>31.75</t>
         </is>
       </c>
-      <c r="R10" s="88" t="inlineStr">
+      <c r="S10" s="88" t="inlineStr">
         <is>
           <t>31.00</t>
         </is>
       </c>
-      <c r="S10" s="88" t="inlineStr">
+      <c r="T10" s="88" t="inlineStr">
         <is>
           <t>30.50</t>
         </is>
       </c>
-      <c r="T10" s="88" t="inlineStr">
+      <c r="U10" s="88" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="U10" s="88" t="inlineStr">
+      <c r="V10" s="88" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="V10" s="88" t="inlineStr">
+      <c r="W10" s="88" t="inlineStr">
         <is>
           <t>29.25</t>
         </is>
       </c>
-      <c r="W10" s="88" t="inlineStr">
+      <c r="X10" s="88" t="inlineStr">
         <is>
           <t>28.25</t>
         </is>
       </c>
-      <c r="X10" s="88" t="inlineStr">
+      <c r="Y10" s="88" t="inlineStr">
         <is>
           <t>27.25</t>
         </is>
       </c>
-      <c r="Y10" s="88" t="inlineStr">
+      <c r="Z10" s="88" t="inlineStr">
         <is>
           <t>26.50</t>
         </is>
       </c>
-      <c r="Z10" s="88" t="inlineStr">
+      <c r="AA10" s="88" t="inlineStr">
         <is>
           <t>25.75</t>
         </is>
       </c>
-      <c r="AA10" s="88" t="inlineStr">
+      <c r="AB10" s="89" t="inlineStr">
         <is>
           <t>25.00</t>
         </is>
       </c>
-      <c r="AB10" s="89" t="n"/>
     </row>
     <row customHeight="1" ht="37.5" r="11">
       <c r="A11" s="1" t="n"/>
@@ -2209,752 +2249,800 @@
       <c r="B12" s="4" t="n"/>
       <c r="C12" s="58" t="inlineStr">
         <is>
+          <t>Safe Cover</t>
+        </is>
+      </c>
+      <c r="D12" s="36" t="inlineStr">
+        <is>
           <t>23.50</t>
         </is>
       </c>
-      <c r="D12" s="36" t="inlineStr">
+      <c r="E12" s="36" t="inlineStr">
         <is>
           <t>23.00</t>
         </is>
       </c>
-      <c r="E12" s="36" t="inlineStr">
+      <c r="F12" s="36" t="inlineStr">
         <is>
           <t>21.75</t>
         </is>
       </c>
-      <c r="F12" s="36" t="inlineStr">
+      <c r="G12" s="28" t="inlineStr">
         <is>
           <t>21.00</t>
         </is>
       </c>
-      <c r="G12" s="28" t="n"/>
       <c r="H12" s="73" t="inlineStr">
         <is>
+          <t>Safe Cover</t>
+        </is>
+      </c>
+      <c r="I12" s="27" t="inlineStr">
+        <is>
           <t>47.50</t>
         </is>
       </c>
-      <c r="I12" s="27" t="inlineStr">
+      <c r="J12" s="27" t="inlineStr">
         <is>
           <t>41.25</t>
         </is>
       </c>
-      <c r="J12" s="27" t="inlineStr">
+      <c r="K12" s="27" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="K12" s="27" t="inlineStr">
+      <c r="L12" s="27" t="inlineStr">
         <is>
           <t>35.75</t>
         </is>
       </c>
-      <c r="L12" s="27" t="inlineStr">
+      <c r="M12" s="27" t="inlineStr">
         <is>
           <t>34.50</t>
         </is>
       </c>
-      <c r="M12" s="27" t="inlineStr">
+      <c r="N12" s="27" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="N12" s="27" t="inlineStr">
+      <c r="O12" s="27" t="inlineStr">
         <is>
           <t>32.50</t>
         </is>
       </c>
-      <c r="O12" s="27" t="inlineStr">
+      <c r="P12" s="27" t="inlineStr">
         <is>
           <t>32.25</t>
         </is>
       </c>
-      <c r="P12" s="27" t="inlineStr">
+      <c r="Q12" s="27" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="Q12" s="27" t="inlineStr">
+      <c r="R12" s="27" t="inlineStr">
         <is>
           <t>30.75</t>
         </is>
       </c>
-      <c r="R12" s="27" t="inlineStr">
+      <c r="S12" s="27" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="S12" s="27" t="inlineStr">
+      <c r="T12" s="27" t="inlineStr">
         <is>
           <t>29.50</t>
         </is>
       </c>
-      <c r="T12" s="27" t="inlineStr">
+      <c r="U12" s="27" t="inlineStr">
         <is>
           <t>29.00</t>
         </is>
       </c>
-      <c r="U12" s="27" t="inlineStr">
+      <c r="V12" s="27" t="inlineStr">
         <is>
           <t>28.75</t>
         </is>
       </c>
-      <c r="V12" s="27" t="inlineStr">
+      <c r="W12" s="27" t="inlineStr">
         <is>
           <t>28.25</t>
         </is>
       </c>
-      <c r="W12" s="27" t="inlineStr">
+      <c r="X12" s="27" t="inlineStr">
         <is>
           <t>27.25</t>
         </is>
       </c>
-      <c r="X12" s="27" t="inlineStr">
+      <c r="Y12" s="27" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="Y12" s="27" t="inlineStr">
+      <c r="Z12" s="27" t="inlineStr">
         <is>
           <t>25.50</t>
         </is>
       </c>
-      <c r="Z12" s="27" t="inlineStr">
+      <c r="AA12" s="27" t="inlineStr">
         <is>
           <t>24.75</t>
         </is>
       </c>
-      <c r="AA12" s="27" t="inlineStr">
+      <c r="AB12" s="28" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="AB12" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="13">
       <c r="B13" s="4" t="n"/>
       <c r="C13" s="53" t="inlineStr">
         <is>
+          <t>Clean Wood Chips</t>
+        </is>
+      </c>
+      <c r="D13" s="35" t="inlineStr">
+        <is>
           <t>23.50</t>
         </is>
       </c>
-      <c r="D13" s="35" t="inlineStr">
+      <c r="E13" s="35" t="inlineStr">
         <is>
           <t>23.00</t>
         </is>
       </c>
-      <c r="E13" s="35" t="inlineStr">
+      <c r="F13" s="35" t="inlineStr">
         <is>
           <t>21.75</t>
         </is>
       </c>
-      <c r="F13" s="35" t="inlineStr">
+      <c r="G13" s="22" t="inlineStr">
         <is>
           <t>21.00</t>
         </is>
       </c>
-      <c r="G13" s="22" t="n"/>
       <c r="H13" s="68" t="inlineStr">
         <is>
+          <t>Clean Wood Chips</t>
+        </is>
+      </c>
+      <c r="I13" s="21" t="inlineStr">
+        <is>
           <t>47.50</t>
         </is>
       </c>
-      <c r="I13" s="21" t="inlineStr">
+      <c r="J13" s="21" t="inlineStr">
         <is>
           <t>41.25</t>
         </is>
       </c>
-      <c r="J13" s="21" t="inlineStr">
+      <c r="K13" s="21" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="K13" s="21" t="inlineStr">
+      <c r="L13" s="21" t="inlineStr">
         <is>
           <t>35.75</t>
         </is>
       </c>
-      <c r="L13" s="21" t="inlineStr">
+      <c r="M13" s="21" t="inlineStr">
         <is>
           <t>34.50</t>
         </is>
       </c>
-      <c r="M13" s="21" t="inlineStr">
+      <c r="N13" s="21" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="N13" s="21" t="inlineStr">
+      <c r="O13" s="21" t="inlineStr">
         <is>
           <t>32.50</t>
         </is>
       </c>
-      <c r="O13" s="21" t="inlineStr">
+      <c r="P13" s="21" t="inlineStr">
         <is>
           <t>32.25</t>
         </is>
       </c>
-      <c r="P13" s="21" t="inlineStr">
+      <c r="Q13" s="21" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="Q13" s="21" t="inlineStr">
+      <c r="R13" s="21" t="inlineStr">
         <is>
           <t>30.75</t>
         </is>
       </c>
-      <c r="R13" s="21" t="inlineStr">
+      <c r="S13" s="21" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="S13" s="21" t="inlineStr">
+      <c r="T13" s="21" t="inlineStr">
         <is>
           <t>29.50</t>
         </is>
       </c>
-      <c r="T13" s="21" t="inlineStr">
+      <c r="U13" s="21" t="inlineStr">
         <is>
           <t>29.00</t>
         </is>
       </c>
-      <c r="U13" s="21" t="inlineStr">
+      <c r="V13" s="21" t="inlineStr">
         <is>
           <t>28.75</t>
         </is>
       </c>
-      <c r="V13" s="21" t="inlineStr">
+      <c r="W13" s="21" t="inlineStr">
         <is>
           <t>28.25</t>
         </is>
       </c>
-      <c r="W13" s="21" t="inlineStr">
+      <c r="X13" s="21" t="inlineStr">
         <is>
           <t>27.25</t>
         </is>
       </c>
-      <c r="X13" s="21" t="inlineStr">
+      <c r="Y13" s="21" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="Y13" s="21" t="inlineStr">
+      <c r="Z13" s="21" t="inlineStr">
         <is>
           <t>25.50</t>
         </is>
       </c>
-      <c r="Z13" s="21" t="inlineStr">
+      <c r="AA13" s="21" t="inlineStr">
         <is>
           <t>24.75</t>
         </is>
       </c>
-      <c r="AA13" s="21" t="inlineStr">
+      <c r="AB13" s="22" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="AB13" s="22" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="6" t="n"/>
       <c r="C14" s="52" t="inlineStr">
         <is>
+          <t>Wood Chips</t>
+        </is>
+      </c>
+      <c r="D14" s="34" t="inlineStr">
+        <is>
           <t>11.75</t>
         </is>
       </c>
-      <c r="D14" s="34" t="inlineStr">
+      <c r="E14" s="34" t="inlineStr">
         <is>
           <t>11.50</t>
         </is>
       </c>
-      <c r="E14" s="34" t="inlineStr">
+      <c r="F14" s="34" t="inlineStr">
         <is>
           <t>10.75</t>
         </is>
       </c>
-      <c r="F14" s="34" t="inlineStr">
+      <c r="G14" s="20" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="G14" s="20" t="n"/>
       <c r="H14" s="67" t="inlineStr">
         <is>
+          <t>Wood Chips</t>
+        </is>
+      </c>
+      <c r="I14" s="19" t="inlineStr">
+        <is>
           <t>35.75</t>
         </is>
       </c>
-      <c r="I14" s="19" t="inlineStr">
+      <c r="J14" s="19" t="inlineStr">
         <is>
           <t>29.50</t>
         </is>
       </c>
-      <c r="J14" s="19" t="inlineStr">
+      <c r="K14" s="19" t="inlineStr">
         <is>
           <t>26.00</t>
         </is>
       </c>
-      <c r="K14" s="19" t="inlineStr">
+      <c r="L14" s="19" t="inlineStr">
         <is>
           <t>24.25</t>
         </is>
       </c>
-      <c r="L14" s="19" t="inlineStr">
+      <c r="M14" s="19" t="inlineStr">
         <is>
           <t>23.00</t>
         </is>
       </c>
-      <c r="M14" s="19" t="inlineStr">
+      <c r="N14" s="19" t="inlineStr">
         <is>
           <t>22.00</t>
         </is>
       </c>
-      <c r="N14" s="19" t="inlineStr">
+      <c r="O14" s="19" t="inlineStr">
         <is>
           <t>21.75</t>
         </is>
       </c>
-      <c r="O14" s="19" t="inlineStr">
+      <c r="P14" s="19" t="inlineStr">
         <is>
           <t>21.50</t>
         </is>
       </c>
-      <c r="P14" s="19" t="inlineStr">
+      <c r="Q14" s="19" t="inlineStr">
         <is>
           <t>21.00</t>
         </is>
       </c>
-      <c r="Q14" s="19" t="inlineStr">
+      <c r="R14" s="19" t="inlineStr">
         <is>
           <t>20.25</t>
         </is>
       </c>
-      <c r="R14" s="19" t="inlineStr">
+      <c r="S14" s="19" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="S14" s="19" t="inlineStr">
+      <c r="T14" s="19" t="inlineStr">
         <is>
           <t>19.00</t>
         </is>
       </c>
-      <c r="T14" s="19" t="inlineStr">
+      <c r="U14" s="19" t="inlineStr">
         <is>
           <t>18.50</t>
         </is>
       </c>
-      <c r="U14" s="19" t="inlineStr">
+      <c r="V14" s="19" t="inlineStr">
         <is>
           <t>18.25</t>
         </is>
       </c>
-      <c r="V14" s="19" t="inlineStr">
+      <c r="W14" s="19" t="inlineStr">
         <is>
           <t>17.75</t>
         </is>
       </c>
-      <c r="W14" s="19" t="inlineStr">
+      <c r="X14" s="19" t="inlineStr">
         <is>
           <t>16.75</t>
         </is>
       </c>
-      <c r="X14" s="19" t="inlineStr">
+      <c r="Y14" s="19" t="inlineStr">
         <is>
           <t>15.75</t>
         </is>
       </c>
-      <c r="Y14" s="19" t="inlineStr">
+      <c r="Z14" s="19" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="Z14" s="19" t="inlineStr">
+      <c r="AA14" s="19" t="inlineStr">
         <is>
           <t>14.25</t>
         </is>
       </c>
-      <c r="AA14" s="19" t="inlineStr">
+      <c r="AB14" s="20" t="inlineStr">
         <is>
           <t>13.50</t>
         </is>
       </c>
-      <c r="AB14" s="20" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="15">
       <c r="B15" s="4" t="n"/>
       <c r="C15" s="59" t="inlineStr">
         <is>
+          <t>Compost</t>
+        </is>
+      </c>
+      <c r="D15" s="35" t="inlineStr">
+        <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="D15" s="35" t="inlineStr">
+      <c r="E15" s="35" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="E15" s="35" t="inlineStr">
+      <c r="F15" s="35" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="F15" s="35" t="inlineStr">
+      <c r="G15" s="22" t="inlineStr">
         <is>
           <t>25.50</t>
         </is>
       </c>
-      <c r="G15" s="22" t="n"/>
       <c r="H15" s="74" t="inlineStr">
         <is>
+          <t>Compost</t>
+        </is>
+      </c>
+      <c r="I15" s="21" t="inlineStr">
+        <is>
           <t>52.50</t>
         </is>
       </c>
-      <c r="I15" s="21" t="inlineStr">
+      <c r="J15" s="21" t="inlineStr">
         <is>
           <t>46.25</t>
         </is>
       </c>
-      <c r="J15" s="21" t="inlineStr">
+      <c r="K15" s="21" t="inlineStr">
         <is>
           <t>42.50</t>
         </is>
       </c>
-      <c r="K15" s="21" t="inlineStr">
+      <c r="L15" s="21" t="inlineStr">
         <is>
           <t>40.50</t>
         </is>
       </c>
-      <c r="L15" s="21" t="inlineStr">
+      <c r="M15" s="21" t="inlineStr">
         <is>
           <t>39.25</t>
         </is>
       </c>
-      <c r="M15" s="21" t="inlineStr">
+      <c r="N15" s="21" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="N15" s="21" t="inlineStr">
+      <c r="O15" s="21" t="inlineStr">
         <is>
           <t>37.25</t>
         </is>
       </c>
-      <c r="O15" s="21" t="inlineStr">
+      <c r="P15" s="21" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="P15" s="21" t="inlineStr">
+      <c r="Q15" s="21" t="inlineStr">
         <is>
           <t>36.00</t>
         </is>
       </c>
-      <c r="Q15" s="21" t="inlineStr">
+      <c r="R15" s="21" t="inlineStr">
         <is>
           <t>35.25</t>
         </is>
       </c>
-      <c r="R15" s="21" t="inlineStr">
+      <c r="S15" s="21" t="inlineStr">
         <is>
           <t>34.50</t>
         </is>
       </c>
-      <c r="S15" s="21" t="inlineStr">
+      <c r="T15" s="21" t="inlineStr">
         <is>
           <t>34.00</t>
         </is>
       </c>
-      <c r="T15" s="21" t="inlineStr">
+      <c r="U15" s="21" t="inlineStr">
         <is>
           <t>33.50</t>
         </is>
       </c>
-      <c r="U15" s="21" t="inlineStr">
+      <c r="V15" s="21" t="inlineStr">
         <is>
           <t>33.25</t>
         </is>
       </c>
-      <c r="V15" s="21" t="inlineStr">
+      <c r="W15" s="21" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="W15" s="21" t="inlineStr">
+      <c r="X15" s="21" t="inlineStr">
         <is>
           <t>31.75</t>
         </is>
       </c>
-      <c r="X15" s="21" t="inlineStr">
+      <c r="Y15" s="21" t="inlineStr">
         <is>
           <t>30.75</t>
         </is>
       </c>
-      <c r="Y15" s="21" t="inlineStr">
+      <c r="Z15" s="21" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="Z15" s="21" t="inlineStr">
+      <c r="AA15" s="21" t="inlineStr">
         <is>
           <t>29.25</t>
         </is>
       </c>
-      <c r="AA15" s="21" t="inlineStr">
+      <c r="AB15" s="22" t="inlineStr">
         <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="AB15" s="22" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="16">
       <c r="B16" s="4" t="n"/>
       <c r="C16" s="52" t="inlineStr">
         <is>
+          <t>Leaf Compost</t>
+        </is>
+      </c>
+      <c r="D16" s="34" t="inlineStr">
+        <is>
           <t>17.25</t>
         </is>
       </c>
-      <c r="D16" s="34" t="inlineStr">
+      <c r="E16" s="34" t="inlineStr">
         <is>
           <t>17.00</t>
         </is>
       </c>
-      <c r="E16" s="34" t="inlineStr">
+      <c r="F16" s="34" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="F16" s="34" t="inlineStr">
+      <c r="G16" s="20" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="G16" s="20" t="n"/>
       <c r="H16" s="67" t="inlineStr">
         <is>
+          <t>Leaf Compost</t>
+        </is>
+      </c>
+      <c r="I16" s="19" t="inlineStr">
+        <is>
           <t>41.25</t>
         </is>
       </c>
-      <c r="I16" s="19" t="inlineStr">
+      <c r="J16" s="19" t="inlineStr">
         <is>
           <t>35.00</t>
         </is>
       </c>
-      <c r="J16" s="19" t="inlineStr">
+      <c r="K16" s="19" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="K16" s="19" t="inlineStr">
+      <c r="L16" s="19" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="L16" s="19" t="inlineStr">
+      <c r="M16" s="19" t="inlineStr">
         <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="M16" s="19" t="inlineStr">
+      <c r="N16" s="19" t="inlineStr">
         <is>
           <t>27.25</t>
         </is>
       </c>
-      <c r="N16" s="19" t="inlineStr">
+      <c r="O16" s="19" t="inlineStr">
         <is>
           <t>26.75</t>
         </is>
       </c>
-      <c r="O16" s="19" t="inlineStr">
+      <c r="P16" s="19" t="inlineStr">
         <is>
           <t>26.75</t>
         </is>
       </c>
-      <c r="P16" s="19" t="inlineStr">
+      <c r="Q16" s="19" t="inlineStr">
         <is>
           <t>26.00</t>
         </is>
       </c>
-      <c r="Q16" s="19" t="inlineStr">
+      <c r="R16" s="19" t="inlineStr">
         <is>
           <t>25.25</t>
         </is>
       </c>
-      <c r="R16" s="19" t="inlineStr">
+      <c r="S16" s="19" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="S16" s="19" t="inlineStr">
+      <c r="T16" s="19" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="T16" s="19" t="inlineStr">
+      <c r="U16" s="19" t="inlineStr">
         <is>
           <t>23.50</t>
         </is>
       </c>
-      <c r="U16" s="19" t="inlineStr">
+      <c r="V16" s="19" t="inlineStr">
         <is>
           <t>23.25</t>
         </is>
       </c>
-      <c r="V16" s="19" t="inlineStr">
+      <c r="W16" s="19" t="inlineStr">
         <is>
           <t>22.75</t>
         </is>
       </c>
-      <c r="W16" s="19" t="inlineStr">
+      <c r="X16" s="19" t="inlineStr">
         <is>
           <t>21.75</t>
         </is>
       </c>
-      <c r="X16" s="19" t="inlineStr">
+      <c r="Y16" s="19" t="inlineStr">
         <is>
           <t>20.75</t>
         </is>
       </c>
-      <c r="Y16" s="19" t="inlineStr">
+      <c r="Z16" s="19" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="Z16" s="19" t="inlineStr">
+      <c r="AA16" s="19" t="inlineStr">
         <is>
           <t>19.25</t>
         </is>
       </c>
-      <c r="AA16" s="19" t="inlineStr">
+      <c r="AB16" s="20" t="inlineStr">
         <is>
           <t>18.50</t>
         </is>
       </c>
-      <c r="AB16" s="20" t="n"/>
     </row>
     <row customHeight="1" ht="75" r="17">
       <c r="B17" s="4" t="n"/>
       <c r="C17" s="60" t="inlineStr">
         <is>
+          <t>Mushroom Soil</t>
+        </is>
+      </c>
+      <c r="D17" s="37" t="inlineStr">
+        <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="D17" s="37" t="inlineStr">
+      <c r="E17" s="37" t="inlineStr">
         <is>
           <t>9.75</t>
         </is>
       </c>
-      <c r="E17" s="37" t="inlineStr">
+      <c r="F17" s="37" t="inlineStr">
         <is>
           <t>9.25</t>
         </is>
       </c>
-      <c r="F17" s="37" t="inlineStr">
+      <c r="G17" s="31" t="inlineStr">
         <is>
           <t>9.00</t>
         </is>
       </c>
-      <c r="G17" s="31" t="n"/>
       <c r="H17" s="68" t="inlineStr">
         <is>
+          <t>Mushroom Soil</t>
+        </is>
+      </c>
+      <c r="I17" s="29" t="inlineStr">
+        <is>
           <t>34.00</t>
         </is>
       </c>
-      <c r="I17" s="29" t="inlineStr">
+      <c r="J17" s="29" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="J17" s="29" t="inlineStr">
+      <c r="K17" s="29" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="K17" s="29" t="inlineStr">
+      <c r="L17" s="29" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="L17" s="29" t="inlineStr">
+      <c r="M17" s="29" t="inlineStr">
         <is>
           <t>21.25</t>
         </is>
       </c>
-      <c r="M17" s="29" t="inlineStr">
+      <c r="N17" s="29" t="inlineStr">
         <is>
           <t>20.50</t>
         </is>
       </c>
-      <c r="N17" s="29" t="inlineStr">
+      <c r="O17" s="29" t="inlineStr">
         <is>
           <t>20.25</t>
         </is>
       </c>
-      <c r="O17" s="29" t="inlineStr">
+      <c r="P17" s="29" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="P17" s="29" t="inlineStr">
+      <c r="Q17" s="29" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="Q17" s="29" t="inlineStr">
+      <c r="R17" s="29" t="inlineStr">
         <is>
           <t>18.75</t>
         </is>
       </c>
-      <c r="R17" s="29" t="inlineStr">
+      <c r="S17" s="29" t="inlineStr">
         <is>
           <t>18.00</t>
         </is>
       </c>
-      <c r="S17" s="29" t="inlineStr">
+      <c r="T17" s="29" t="inlineStr">
         <is>
           <t>17.50</t>
         </is>
       </c>
-      <c r="T17" s="29" t="inlineStr">
+      <c r="U17" s="29" t="inlineStr">
         <is>
           <t>17.00</t>
         </is>
       </c>
-      <c r="U17" s="29" t="inlineStr">
+      <c r="V17" s="29" t="inlineStr">
         <is>
           <t>16.75</t>
         </is>
       </c>
-      <c r="V17" s="29" t="inlineStr">
+      <c r="W17" s="29" t="inlineStr">
         <is>
           <t>16.25</t>
         </is>
       </c>
-      <c r="W17" s="29" t="inlineStr">
+      <c r="X17" s="29" t="inlineStr">
         <is>
           <t>15.25</t>
         </is>
       </c>
-      <c r="X17" s="29" t="inlineStr">
+      <c r="Y17" s="30" t="inlineStr">
         <is>
           <t>14.25</t>
         </is>
       </c>
-      <c r="Y17" s="30" t="inlineStr">
+      <c r="Z17" s="30" t="inlineStr">
         <is>
           <t>13.50</t>
         </is>
       </c>
-      <c r="Z17" s="30" t="inlineStr">
+      <c r="AA17" s="30" t="inlineStr">
         <is>
           <t>12.75</t>
         </is>
       </c>
-      <c r="AA17" s="30" t="inlineStr">
+      <c r="AB17" s="31" t="inlineStr">
         <is>
           <t>12.00</t>
         </is>
       </c>
-      <c r="AB17" s="31" t="n"/>
     </row>
     <row customHeight="1" ht="37.5" r="18">
       <c r="B18" s="4" t="n"/>
@@ -3031,106 +3119,114 @@
       <c r="B19" s="4" t="n"/>
       <c r="C19" s="62" t="inlineStr">
         <is>
+          <t>Rain Garden Mix</t>
+        </is>
+      </c>
+      <c r="D19" s="37" t="inlineStr">
+        <is>
           <t>30.75</t>
         </is>
       </c>
-      <c r="D19" s="37" t="inlineStr">
+      <c r="E19" s="37" t="inlineStr">
         <is>
           <t>30.00</t>
         </is>
       </c>
-      <c r="E19" s="37" t="inlineStr">
+      <c r="F19" s="37" t="inlineStr">
         <is>
           <t>28.25</t>
         </is>
       </c>
-      <c r="F19" s="37" t="inlineStr">
+      <c r="G19" s="30" t="inlineStr">
         <is>
           <t>27.50</t>
         </is>
       </c>
-      <c r="G19" s="30" t="n"/>
       <c r="H19" s="76" t="inlineStr">
         <is>
+          <t>Rain Garden Mix</t>
+        </is>
+      </c>
+      <c r="I19" s="38" t="inlineStr">
+        <is>
           <t>57.75</t>
         </is>
       </c>
-      <c r="I19" s="38" t="inlineStr">
+      <c r="J19" s="38" t="inlineStr">
         <is>
           <t>51.25</t>
         </is>
       </c>
-      <c r="J19" s="38" t="inlineStr">
+      <c r="K19" s="38" t="inlineStr">
         <is>
           <t>47.50</t>
         </is>
       </c>
-      <c r="K19" s="38" t="inlineStr">
+      <c r="L19" s="38" t="inlineStr">
         <is>
           <t>45.75</t>
         </is>
       </c>
-      <c r="L19" s="38" t="inlineStr">
+      <c r="M19" s="38" t="inlineStr">
         <is>
           <t>44.50</t>
         </is>
       </c>
-      <c r="M19" s="38" t="inlineStr">
+      <c r="N19" s="38" t="inlineStr">
         <is>
           <t>42.25</t>
         </is>
       </c>
-      <c r="N19" s="38" t="inlineStr">
+      <c r="O19" s="38" t="inlineStr">
         <is>
           <t>41.50</t>
         </is>
       </c>
-      <c r="O19" s="38" t="inlineStr">
+      <c r="P19" s="38" t="inlineStr">
         <is>
           <t>40.50</t>
         </is>
       </c>
-      <c r="P19" s="38" t="inlineStr">
+      <c r="Q19" s="38" t="inlineStr">
         <is>
           <t>38.75</t>
         </is>
       </c>
-      <c r="Q19" s="38" t="inlineStr">
+      <c r="R19" s="38" t="inlineStr">
         <is>
           <t>38.25</t>
         </is>
       </c>
-      <c r="R19" s="38" t="inlineStr">
+      <c r="S19" s="38" t="inlineStr">
         <is>
           <t>37.50</t>
         </is>
       </c>
-      <c r="S19" s="38" t="inlineStr">
+      <c r="T19" s="38" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="T19" s="38" t="inlineStr">
+      <c r="U19" s="38" t="inlineStr">
         <is>
           <t>36.75</t>
         </is>
       </c>
-      <c r="U19" s="38" t="inlineStr">
+      <c r="V19" s="38" t="inlineStr">
         <is>
           <t>36.25</t>
         </is>
       </c>
-      <c r="V19" s="38" t="inlineStr">
+      <c r="W19" s="38" t="inlineStr">
         <is>
           <t>36.25</t>
         </is>
       </c>
-      <c r="W19" s="38" t="inlineStr">
+      <c r="X19" s="42" t="inlineStr">
         <is>
           <t>35.00</t>
         </is>
       </c>
-      <c r="X19" s="42" t="n"/>
       <c r="Y19" s="9" t="n"/>
       <c r="Z19" s="9" t="n"/>
       <c r="AA19" s="9" t="n"/>
@@ -3141,106 +3237,114 @@
       <c r="B20" s="6" t="n"/>
       <c r="C20" s="63" t="inlineStr">
         <is>
+          <t>Screened Blend</t>
+        </is>
+      </c>
+      <c r="D20" s="36" t="inlineStr">
+        <is>
           <t>27.00</t>
         </is>
       </c>
-      <c r="D20" s="36" t="inlineStr">
+      <c r="E20" s="36" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="E20" s="36" t="inlineStr">
+      <c r="F20" s="36" t="inlineStr">
         <is>
           <t>24.75</t>
         </is>
       </c>
-      <c r="F20" s="36" t="inlineStr">
+      <c r="G20" s="27" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="G20" s="27" t="n"/>
       <c r="H20" s="77" t="inlineStr">
         <is>
+          <t>Screened Blend</t>
+        </is>
+      </c>
+      <c r="I20" s="34" t="inlineStr">
+        <is>
           <t>54.00</t>
         </is>
       </c>
-      <c r="I20" s="34" t="inlineStr">
+      <c r="J20" s="34" t="inlineStr">
         <is>
           <t>47.25</t>
         </is>
       </c>
-      <c r="J20" s="34" t="inlineStr">
+      <c r="K20" s="34" t="inlineStr">
         <is>
           <t>43.75</t>
         </is>
       </c>
-      <c r="K20" s="34" t="inlineStr">
+      <c r="L20" s="34" t="inlineStr">
         <is>
           <t>42.00</t>
         </is>
       </c>
-      <c r="L20" s="34" t="inlineStr">
+      <c r="M20" s="34" t="inlineStr">
         <is>
           <t>40.75</t>
         </is>
       </c>
-      <c r="M20" s="34" t="inlineStr">
+      <c r="N20" s="34" t="inlineStr">
         <is>
           <t>38.50</t>
         </is>
       </c>
-      <c r="N20" s="34" t="inlineStr">
+      <c r="O20" s="34" t="inlineStr">
         <is>
           <t>38.00</t>
         </is>
       </c>
-      <c r="O20" s="34" t="inlineStr">
+      <c r="P20" s="34" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="P20" s="34" t="inlineStr">
+      <c r="Q20" s="34" t="inlineStr">
         <is>
           <t>35.25</t>
         </is>
       </c>
-      <c r="Q20" s="34" t="inlineStr">
+      <c r="R20" s="34" t="inlineStr">
         <is>
           <t>34.75</t>
         </is>
       </c>
-      <c r="R20" s="34" t="inlineStr">
+      <c r="S20" s="34" t="inlineStr">
         <is>
           <t>34.00</t>
         </is>
       </c>
-      <c r="S20" s="34" t="inlineStr">
+      <c r="T20" s="34" t="inlineStr">
         <is>
           <t>33.50</t>
         </is>
       </c>
-      <c r="T20" s="34" t="inlineStr">
+      <c r="U20" s="34" t="inlineStr">
         <is>
           <t>33.25</t>
         </is>
       </c>
-      <c r="U20" s="34" t="inlineStr">
+      <c r="V20" s="34" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="V20" s="34" t="inlineStr">
+      <c r="W20" s="34" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="W20" s="34" t="inlineStr">
+      <c r="X20" s="20" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="X20" s="20" t="n"/>
       <c r="Y20" s="9" t="n"/>
       <c r="Z20" s="9" t="n"/>
       <c r="AA20" s="9" t="n"/>
@@ -3250,106 +3354,114 @@
       <c r="B21" s="4" t="n"/>
       <c r="C21" s="64" t="inlineStr">
         <is>
+          <t>Screened Topsoil</t>
+        </is>
+      </c>
+      <c r="D21" s="38" t="inlineStr">
+        <is>
           <t>27.00</t>
         </is>
       </c>
-      <c r="D21" s="38" t="inlineStr">
+      <c r="E21" s="38" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="E21" s="38" t="inlineStr">
+      <c r="F21" s="38" t="inlineStr">
         <is>
           <t>24.75</t>
         </is>
       </c>
-      <c r="F21" s="38" t="inlineStr">
+      <c r="G21" s="39" t="inlineStr">
         <is>
           <t>24.00</t>
         </is>
       </c>
-      <c r="G21" s="39" t="n"/>
       <c r="H21" s="64" t="inlineStr">
         <is>
+          <t>Screened Topsoil</t>
+        </is>
+      </c>
+      <c r="I21" s="34" t="inlineStr">
+        <is>
           <t>54.00</t>
         </is>
       </c>
-      <c r="I21" s="34" t="inlineStr">
+      <c r="J21" s="34" t="inlineStr">
         <is>
           <t>47.25</t>
         </is>
       </c>
-      <c r="J21" s="34" t="inlineStr">
+      <c r="K21" s="34" t="inlineStr">
         <is>
           <t>43.75</t>
         </is>
       </c>
-      <c r="K21" s="34" t="inlineStr">
+      <c r="L21" s="34" t="inlineStr">
         <is>
           <t>42.00</t>
         </is>
       </c>
-      <c r="L21" s="34" t="inlineStr">
+      <c r="M21" s="34" t="inlineStr">
         <is>
           <t>40.75</t>
         </is>
       </c>
-      <c r="M21" s="34" t="inlineStr">
+      <c r="N21" s="34" t="inlineStr">
         <is>
           <t>38.50</t>
         </is>
       </c>
-      <c r="N21" s="34" t="inlineStr">
+      <c r="O21" s="34" t="inlineStr">
         <is>
           <t>38.00</t>
         </is>
       </c>
-      <c r="O21" s="34" t="inlineStr">
+      <c r="P21" s="34" t="inlineStr">
         <is>
           <t>37.00</t>
         </is>
       </c>
-      <c r="P21" s="34" t="inlineStr">
+      <c r="Q21" s="34" t="inlineStr">
         <is>
           <t>35.25</t>
         </is>
       </c>
-      <c r="Q21" s="34" t="inlineStr">
+      <c r="R21" s="34" t="inlineStr">
         <is>
           <t>34.75</t>
         </is>
       </c>
-      <c r="R21" s="34" t="inlineStr">
+      <c r="S21" s="34" t="inlineStr">
         <is>
           <t>34.00</t>
         </is>
       </c>
-      <c r="S21" s="34" t="inlineStr">
+      <c r="T21" s="34" t="inlineStr">
         <is>
           <t>33.50</t>
         </is>
       </c>
-      <c r="T21" s="34" t="inlineStr">
+      <c r="U21" s="34" t="inlineStr">
         <is>
           <t>33.25</t>
         </is>
       </c>
-      <c r="U21" s="34" t="inlineStr">
+      <c r="V21" s="34" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="V21" s="34" t="inlineStr">
+      <c r="W21" s="34" t="inlineStr">
         <is>
           <t>32.75</t>
         </is>
       </c>
-      <c r="W21" s="34" t="inlineStr">
+      <c r="X21" s="20" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="X21" s="20" t="n"/>
       <c r="Y21" s="9" t="n"/>
       <c r="Z21" s="9" t="n"/>
       <c r="AA21" s="9" t="n"/>
@@ -3359,106 +3471,114 @@
       <c r="B22" s="4" t="n"/>
       <c r="C22" s="52" t="inlineStr">
         <is>
+          <t>Topsoil</t>
+        </is>
+      </c>
+      <c r="D22" s="36" t="inlineStr">
+        <is>
           <t>19.00</t>
         </is>
       </c>
-      <c r="D22" s="36" t="inlineStr">
+      <c r="E22" s="36" t="inlineStr">
         <is>
           <t>18.50</t>
         </is>
       </c>
-      <c r="E22" s="36" t="inlineStr">
+      <c r="F22" s="36" t="inlineStr">
         <is>
           <t>17.50</t>
         </is>
       </c>
-      <c r="F22" s="36" t="inlineStr">
+      <c r="G22" s="27" t="inlineStr">
         <is>
           <t>17.00</t>
         </is>
       </c>
-      <c r="G22" s="27" t="n"/>
       <c r="H22" s="52" t="inlineStr">
         <is>
+          <t>Topsoil</t>
+        </is>
+      </c>
+      <c r="I22" s="34" t="inlineStr">
+        <is>
           <t>46.00</t>
         </is>
       </c>
-      <c r="I22" s="34" t="inlineStr">
+      <c r="J22" s="34" t="inlineStr">
         <is>
           <t>39.25</t>
         </is>
       </c>
-      <c r="J22" s="34" t="inlineStr">
+      <c r="K22" s="34" t="inlineStr">
         <is>
           <t>36.00</t>
         </is>
       </c>
-      <c r="K22" s="34" t="inlineStr">
+      <c r="L22" s="34" t="inlineStr">
         <is>
           <t>34.25</t>
         </is>
       </c>
-      <c r="L22" s="34" t="inlineStr">
+      <c r="M22" s="34" t="inlineStr">
         <is>
           <t>33.25</t>
         </is>
       </c>
-      <c r="M22" s="34" t="inlineStr">
+      <c r="N22" s="34" t="inlineStr">
         <is>
           <t>31.25</t>
         </is>
       </c>
-      <c r="N22" s="34" t="inlineStr">
+      <c r="O22" s="34" t="inlineStr">
         <is>
           <t>30.75</t>
         </is>
       </c>
-      <c r="O22" s="34" t="inlineStr">
+      <c r="P22" s="34" t="inlineStr">
         <is>
           <t>29.75</t>
         </is>
       </c>
-      <c r="P22" s="34" t="inlineStr">
+      <c r="Q22" s="34" t="inlineStr">
         <is>
           <t>28.25</t>
         </is>
       </c>
-      <c r="Q22" s="34" t="inlineStr">
+      <c r="R22" s="34" t="inlineStr">
         <is>
           <t>27.75</t>
         </is>
       </c>
-      <c r="R22" s="34" t="inlineStr">
+      <c r="S22" s="34" t="inlineStr">
         <is>
           <t>27.00</t>
         </is>
       </c>
-      <c r="S22" s="34" t="inlineStr">
+      <c r="T22" s="34" t="inlineStr">
         <is>
           <t>26.50</t>
         </is>
       </c>
-      <c r="T22" s="34" t="inlineStr">
+      <c r="U22" s="34" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="U22" s="34" t="inlineStr">
+      <c r="V22" s="34" t="inlineStr">
         <is>
           <t>25.75</t>
         </is>
       </c>
-      <c r="V22" s="34" t="inlineStr">
+      <c r="W22" s="34" t="inlineStr">
         <is>
           <t>25.75</t>
         </is>
       </c>
-      <c r="W22" s="34" t="inlineStr">
+      <c r="X22" s="20" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="X22" s="20" t="n"/>
       <c r="Y22" s="9" t="n"/>
       <c r="Z22" s="9" t="n"/>
       <c r="AA22" s="9" t="n"/>
@@ -3468,106 +3588,114 @@
       <c r="B23" s="4" t="n"/>
       <c r="C23" s="59" t="inlineStr">
         <is>
+          <t>Fill Dirt</t>
+        </is>
+      </c>
+      <c r="D23" s="38" t="inlineStr">
+        <is>
           <t>11.25</t>
         </is>
       </c>
-      <c r="D23" s="38" t="inlineStr">
+      <c r="E23" s="38" t="inlineStr">
         <is>
           <t>11.00</t>
         </is>
       </c>
-      <c r="E23" s="38" t="inlineStr">
+      <c r="F23" s="38" t="inlineStr">
         <is>
           <t>10.25</t>
         </is>
       </c>
-      <c r="F23" s="38" t="inlineStr">
+      <c r="G23" s="39" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="G23" s="39" t="n"/>
       <c r="H23" s="59" t="inlineStr">
         <is>
+          <t>Fill Dirt</t>
+        </is>
+      </c>
+      <c r="I23" s="35" t="inlineStr">
+        <is>
           <t>38.25</t>
         </is>
       </c>
-      <c r="I23" s="35" t="inlineStr">
+      <c r="J23" s="35" t="inlineStr">
         <is>
           <t>31.50</t>
         </is>
       </c>
-      <c r="J23" s="35" t="inlineStr">
+      <c r="K23" s="35" t="inlineStr">
         <is>
           <t>28.50</t>
         </is>
       </c>
-      <c r="K23" s="35" t="inlineStr">
+      <c r="L23" s="35" t="inlineStr">
         <is>
           <t>26.75</t>
         </is>
       </c>
-      <c r="L23" s="35" t="inlineStr">
+      <c r="M23" s="35" t="inlineStr">
         <is>
           <t>25.50</t>
         </is>
       </c>
-      <c r="M23" s="35" t="inlineStr">
+      <c r="N23" s="35" t="inlineStr">
         <is>
           <t>24.25</t>
         </is>
       </c>
-      <c r="N23" s="35" t="inlineStr">
+      <c r="O23" s="35" t="inlineStr">
         <is>
           <t>23.50</t>
         </is>
       </c>
-      <c r="O23" s="35" t="inlineStr">
+      <c r="P23" s="35" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="P23" s="35" t="inlineStr">
+      <c r="Q23" s="35" t="inlineStr">
         <is>
           <t>21.25</t>
         </is>
       </c>
-      <c r="Q23" s="35" t="inlineStr">
+      <c r="R23" s="35" t="inlineStr">
         <is>
           <t>20.75</t>
         </is>
       </c>
-      <c r="R23" s="35" t="inlineStr">
+      <c r="S23" s="35" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="S23" s="35" t="inlineStr">
+      <c r="T23" s="35" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="T23" s="35" t="inlineStr">
+      <c r="U23" s="35" t="inlineStr">
         <is>
           <t>19.25</t>
         </is>
       </c>
-      <c r="U23" s="35" t="inlineStr">
+      <c r="V23" s="35" t="inlineStr">
         <is>
           <t>18.75</t>
         </is>
       </c>
-      <c r="V23" s="35" t="inlineStr">
+      <c r="W23" s="35" t="inlineStr">
         <is>
           <t>18.75</t>
         </is>
       </c>
-      <c r="W23" s="35" t="inlineStr">
+      <c r="X23" s="22" t="inlineStr">
         <is>
           <t>17.50</t>
         </is>
       </c>
-      <c r="X23" s="22" t="n"/>
       <c r="Y23" s="9" t="n"/>
       <c r="Z23" s="9" t="n"/>
       <c r="AA23" s="9" t="n"/>
@@ -3578,106 +3706,114 @@
       <c r="B24" s="6" t="n"/>
       <c r="C24" s="65" t="inlineStr">
         <is>
+          <t>Topsoil Overs</t>
+        </is>
+      </c>
+      <c r="D24" s="40" t="inlineStr">
+        <is>
           <t>9.00</t>
         </is>
       </c>
-      <c r="D24" s="40" t="inlineStr">
+      <c r="E24" s="40" t="inlineStr">
         <is>
           <t>8.75</t>
         </is>
       </c>
-      <c r="E24" s="40" t="inlineStr">
+      <c r="F24" s="40" t="inlineStr">
         <is>
           <t>8.25</t>
         </is>
       </c>
-      <c r="F24" s="40" t="inlineStr">
+      <c r="G24" s="41" t="inlineStr">
         <is>
           <t>8.00</t>
         </is>
       </c>
-      <c r="G24" s="41" t="n"/>
       <c r="H24" s="65" t="inlineStr">
         <is>
+          <t>Topsoil Overs</t>
+        </is>
+      </c>
+      <c r="I24" s="40" t="inlineStr">
+        <is>
           <t>36.00</t>
         </is>
       </c>
-      <c r="I24" s="40" t="inlineStr">
+      <c r="J24" s="40" t="inlineStr">
         <is>
           <t>29.25</t>
         </is>
       </c>
-      <c r="J24" s="40" t="inlineStr">
+      <c r="K24" s="40" t="inlineStr">
         <is>
           <t>26.25</t>
         </is>
       </c>
-      <c r="K24" s="40" t="inlineStr">
+      <c r="L24" s="40" t="inlineStr">
         <is>
           <t>24.50</t>
         </is>
       </c>
-      <c r="L24" s="40" t="inlineStr">
+      <c r="M24" s="40" t="inlineStr">
         <is>
           <t>23.25</t>
         </is>
       </c>
-      <c r="M24" s="40" t="inlineStr">
+      <c r="N24" s="40" t="inlineStr">
         <is>
           <t>22.00</t>
         </is>
       </c>
-      <c r="N24" s="40" t="inlineStr">
+      <c r="O24" s="40" t="inlineStr">
         <is>
           <t>21.50</t>
         </is>
       </c>
-      <c r="O24" s="40" t="inlineStr">
+      <c r="P24" s="40" t="inlineStr">
         <is>
           <t>20.50</t>
         </is>
       </c>
-      <c r="P24" s="40" t="inlineStr">
+      <c r="Q24" s="40" t="inlineStr">
         <is>
           <t>19.25</t>
         </is>
       </c>
-      <c r="Q24" s="40" t="inlineStr">
+      <c r="R24" s="40" t="inlineStr">
         <is>
           <t>18.75</t>
         </is>
       </c>
-      <c r="R24" s="40" t="inlineStr">
+      <c r="S24" s="40" t="inlineStr">
         <is>
           <t>18.00</t>
         </is>
       </c>
-      <c r="S24" s="40" t="inlineStr">
+      <c r="T24" s="40" t="inlineStr">
         <is>
           <t>17.50</t>
         </is>
       </c>
-      <c r="T24" s="40" t="inlineStr">
+      <c r="U24" s="40" t="inlineStr">
         <is>
           <t>17.25</t>
         </is>
       </c>
-      <c r="U24" s="40" t="inlineStr">
+      <c r="V24" s="40" t="inlineStr">
         <is>
           <t>16.75</t>
         </is>
       </c>
-      <c r="V24" s="40" t="inlineStr">
+      <c r="W24" s="40" t="inlineStr">
         <is>
           <t>16.75</t>
         </is>
       </c>
-      <c r="W24" s="40" t="inlineStr">
+      <c r="X24" s="43" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="X24" s="43" t="n"/>
       <c r="Y24" s="10" t="n"/>
       <c r="Z24" s="10" t="n"/>
       <c r="AA24" s="10" t="n"/>

</xml_diff>